<commit_message>
Getting closer to fully working
Not in complete working condition, but getting really close.
</commit_message>
<xml_diff>
--- a/output/01_14_stimuli.xlsx
+++ b/output/01_14_stimuli.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>number</t>
   </si>
@@ -49,55 +49,88 @@
     <t>practice</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>book_juice</t>
+  </si>
+  <si>
     <t>can</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>banana_kitty</t>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>balloon_eye</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>block_milk</t>
+  </si>
+  <si>
+    <t>look</t>
+  </si>
+  <si>
+    <t>p4</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>door_leg</t>
+  </si>
+  <si>
+    <t>where</t>
+  </si>
+  <si>
+    <t>book</t>
   </si>
   <si>
     <t>generic</t>
   </si>
   <si>
-    <t>p2</t>
-  </si>
-  <si>
-    <t>where</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>bear_cracker</t>
-  </si>
-  <si>
-    <t>do</t>
-  </si>
-  <si>
-    <t>p3</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>cheerios_water</t>
-  </si>
-  <si>
-    <t>look</t>
-  </si>
-  <si>
-    <t>p4</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>hair_cup</t>
+    <t>E</t>
+  </si>
+  <si>
+    <t>juice</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>balloon</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>eye</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>block</t>
+  </si>
+  <si>
+    <t>milk</t>
+  </si>
+  <si>
+    <t>door</t>
+  </si>
+  <si>
+    <t>leg</t>
   </si>
 </sst>
 </file>
@@ -433,7 +466,7 @@
   <s:sheetPr>
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
   </s:sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,118 +511,247 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s"/>
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s"/>
       <c r="G2" t="n">
         <v>5</v>
       </c>
       <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
         <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s"/>
+        <v>14</v>
+      </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
         <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s"/>
-      <c r="G3" t="s"/>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s"/>
+        <v>18</v>
+      </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s"/>
-      <c r="G4" t="s"/>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>15</v>
-      </c>
       <c r="K4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s"/>
+        <v>22</v>
+      </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="n">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="n">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="n">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="n">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="n">
         <v>12</v>
       </c>
-      <c r="F5" t="s"/>
-      <c r="G5" t="s"/>
-      <c r="H5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" t="s">
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="n">
         <v>15</v>
       </c>
-      <c r="K5" t="s">
-        <v>17</v>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="n">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the stuff at the bottom of the sheets
Getting closer to being complete
</commit_message>
<xml_diff>
--- a/output/01_14_stimuli.xlsx
+++ b/output/01_14_stimuli.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
   <si>
     <t>number</t>
   </si>
@@ -55,6 +55,9 @@
     <t>book_juice</t>
   </si>
   <si>
+    <t>generic</t>
+  </si>
+  <si>
     <t>can</t>
   </si>
   <si>
@@ -97,9 +100,6 @@
     <t>book</t>
   </si>
   <si>
-    <t>generic</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -131,6 +131,33 @@
   </si>
   <si>
     <t>leg</t>
+  </si>
+  <si>
+    <t>stim details</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>word_type</t>
+  </si>
+  <si>
+    <t>need_audio</t>
+  </si>
+  <si>
+    <t>need_image</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>find images</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>audio</t>
   </si>
 </sst>
 </file>
@@ -466,7 +493,7 @@
   <s:sheetPr>
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
   </s:sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,59 +550,71 @@
       <c r="I2" t="s">
         <v>12</v>
       </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
       </c>
       <c r="K4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -583,19 +622,19 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
         <v>28</v>
       </c>
       <c r="K6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -606,16 +645,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
         <v>30</v>
       </c>
       <c r="K7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -626,16 +665,16 @@
         <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
       </c>
       <c r="K8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -646,16 +685,16 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
         <v>34</v>
       </c>
       <c r="K9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -666,10 +705,10 @@
         <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -680,10 +719,10 @@
         <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -694,10 +733,10 @@
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -708,10 +747,10 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -752,6 +791,98 @@
     <row r="21" spans="1:11">
       <c r="A21" t="n">
         <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="n">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="n">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="n">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" t="n">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" t="n">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="n">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" t="n">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" t="n">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more work towards final product
</commit_message>
<xml_diff>
--- a/output/01_14_stimuli.xlsx
+++ b/output/01_14_stimuli.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>number</t>
   </si>
@@ -49,6 +49,9 @@
     <t>practice</t>
   </si>
   <si>
+    <t>can</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
@@ -58,12 +61,12 @@
     <t>generic</t>
   </si>
   <si>
-    <t>can</t>
-  </si>
-  <si>
     <t>p2</t>
   </si>
   <si>
+    <t>where</t>
+  </si>
+  <si>
     <t>B</t>
   </si>
   <si>
@@ -94,15 +97,15 @@
     <t>door_leg</t>
   </si>
   <si>
-    <t>where</t>
-  </si>
-  <si>
     <t>book</t>
   </si>
   <si>
     <t>E</t>
   </si>
   <si>
+    <t>unique_video</t>
+  </si>
+  <si>
     <t>juice</t>
   </si>
   <si>
@@ -113,6 +116,9 @@
   </si>
   <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>unique_audio</t>
   </si>
   <si>
     <t>eye</t>
@@ -541,20 +547,23 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
       <c r="G2" t="n">
         <v>5</v>
       </c>
       <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
         <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -564,57 +573,66 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -625,16 +643,19 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H6" t="s">
         <v>28</v>
       </c>
+      <c r="J6" t="s">
+        <v>29</v>
+      </c>
       <c r="K6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -642,19 +663,22 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>30</v>
-      </c>
       <c r="K7" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -662,19 +686,22 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="J8" t="s">
+        <v>34</v>
       </c>
       <c r="K8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -682,19 +709,22 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" t="s">
         <v>34</v>
       </c>
       <c r="K9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -702,13 +732,13 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -716,13 +746,13 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -730,13 +760,13 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -744,81 +774,129 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="n">
         <v>9</v>
       </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="n">
         <v>10</v>
       </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="n">
         <v>11</v>
       </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="n">
         <v>12</v>
       </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="n">
         <v>13</v>
       </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="n">
         <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="n">
         <v>15</v>
       </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="n">
         <v>16</v>
       </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E28" t="s">
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G28" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -826,7 +904,7 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -834,7 +912,7 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -842,7 +920,7 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -850,7 +928,7 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -858,7 +936,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -866,7 +944,7 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -874,7 +952,7 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -882,7 +960,7 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add the NA's under duplicate_image_filename
</commit_message>
<xml_diff>
--- a/output/01_14_stimuli.xlsx
+++ b/output/01_14_stimuli.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>number</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>can</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
   <si>
     <t>A</t>
@@ -550,17 +553,20 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
       <c r="G2" t="n">
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K2" t="s">
         <v>11</v>
@@ -568,71 +574,80 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -640,22 +655,25 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -663,22 +681,25 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -686,19 +707,22 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K8" t="s">
         <v>11</v>
@@ -709,22 +733,25 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" t="s">
         <v>35</v>
       </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" t="s">
-        <v>36</v>
-      </c>
-      <c r="J9" t="s">
-        <v>34</v>
-      </c>
       <c r="K9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -732,13 +759,16 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -746,13 +776,16 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -760,13 +793,16 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -774,13 +810,16 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -788,10 +827,13 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -799,10 +841,13 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -810,10 +855,13 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -821,10 +869,13 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -832,10 +883,13 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -843,21 +897,27 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
       </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="n">
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -865,38 +925,41 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E28" t="s">
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -904,7 +967,7 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -912,7 +975,7 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -920,7 +983,7 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -928,7 +991,7 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -936,7 +999,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -944,7 +1007,7 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -952,7 +1015,7 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -960,7 +1023,7 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>